<commit_message>
Updated portfolio project files
</commit_message>
<xml_diff>
--- a/public/One Page Portfolio.xlsx
+++ b/public/One Page Portfolio.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fbe783a61aeb42e8/Desktop/Portfolio/portfolio-dashboard-01/my-portfolio-dashboard/public/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="20" documentId="8_{BD04B964-0A54-4F13-8FA1-08FAD27F2727}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BB37DE73-AE79-48BB-B2D5-7ACA5B88CF9C}"/>
+  <xr:revisionPtr revIDLastSave="21" documentId="8_{BD04B964-0A54-4F13-8FA1-08FAD27F2727}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0BBD2B26-16A6-4FC2-A434-26E5E684F6D9}"/>
   <bookViews>
-    <workbookView xWindow="1980" yWindow="1392" windowWidth="17280" windowHeight="8880" xr2:uid="{C0A14CF0-A9EB-4C7E-B6C9-F2A28BC14ABC}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{C0A14CF0-A9EB-4C7E-B6C9-F2A28BC14ABC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -577,7 +577,7 @@
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -648,8 +648,7 @@
         <v>93158631</v>
       </c>
       <c r="H2" s="11">
-        <f>128+(4*16)</f>
-        <v>192</v>
+        <v>292</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>7</v>
@@ -863,7 +862,7 @@
       </c>
       <c r="H9" s="12">
         <f>SUM(H2:H8)</f>
-        <v>644</v>
+        <v>744</v>
       </c>
       <c r="I9" s="7"/>
       <c r="J9" s="7"/>

</xml_diff>